<commit_message>
[IMP] Python 3.6 deprecated + no more depends on os0
</commit_message>
<xml_diff>
--- a/z0bug_odoo/data/res_partner.xlsx
+++ b/z0bug_odoo/data/res_partner.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="276">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -166,6 +166,9 @@
     <t xml:space="preserve">https://www.testcompany.org</t>
   </si>
   <si>
+    <t xml:space="preserve">URCROKA</t>
+  </si>
+  <si>
     <t xml:space="preserve">z0bug.partner_mycompany_uk</t>
   </si>
   <si>
@@ -254,6 +257,9 @@
   </si>
   <si>
     <t xml:space="preserve">C. Unità d'Italia, 61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32100</t>
   </si>
   <si>
     <t xml:space="preserve">Belluno</t>
@@ -1074,11 +1080,11 @@
   <dimension ref="A1:AE30"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="Q20" activeCellId="0" sqref="Q20"/>
+      <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="I23" activeCellId="0" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1091,7 +1097,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="6.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="5.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="12.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="10.18"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="6.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="7.75"/>
@@ -1102,7 +1108,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="17.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="18.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="17.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="15.67"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="1" width="15.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="1" width="20.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="1" width="5.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="1" width="8.86"/>
@@ -1327,8 +1333,12 @@
       <c r="U3" s="2"/>
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
+      <c r="X3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="Z3" s="2"/>
       <c r="AA3" s="2"/>
       <c r="AB3" s="2"/>
@@ -1340,18 +1350,18 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="2"/>
@@ -1371,7 +1381,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="2"/>
       <c r="P4" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="Q4" s="2"/>
       <c r="R4" s="2" t="s">
@@ -1390,31 +1400,31 @@
       <c r="AC4" s="2"/>
       <c r="AD4" s="2"/>
       <c r="AE4" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2" t="s">
@@ -1432,7 +1442,7 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="Q5" s="2"/>
       <c r="R5" s="2" t="s">
@@ -1451,23 +1461,23 @@
       <c r="AC5" s="2"/>
       <c r="AD5" s="2"/>
       <c r="AE5" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="2"/>
@@ -1487,7 +1497,7 @@
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="Q6" s="2"/>
       <c r="R6" s="2" t="s">
@@ -1506,29 +1516,29 @@
       <c r="AC6" s="2"/>
       <c r="AD6" s="2"/>
       <c r="AE6" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>42</v>
@@ -1543,27 +1553,27 @@
         <v>43</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O7" s="2"/>
       <c r="P7" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="Q7" s="2"/>
       <c r="R7" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="V7" s="2"/>
       <c r="W7" s="2"/>
@@ -1571,7 +1581,7 @@
         <v>1</v>
       </c>
       <c r="Y7" s="2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="Z7" s="2"/>
       <c r="AA7" s="2"/>
@@ -1584,27 +1594,27 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>67</v>
+        <v>79</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>43</v>
@@ -1616,22 +1626,22 @@
         <v>43</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
       <c r="R8" s="2" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="S8" s="2"/>
       <c r="T8" s="2"/>
       <c r="U8" s="2"/>
       <c r="V8" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="W8" s="2"/>
       <c r="X8" s="2"/>
@@ -1647,27 +1657,27 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J9" s="2" t="s">
         <v>34</v>
@@ -1679,25 +1689,25 @@
         <v>43</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
       <c r="P9" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="R9" s="2"/>
       <c r="S9" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="U9" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="V9" s="2"/>
       <c r="W9" s="2"/>
@@ -1714,29 +1724,29 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>34</v>
@@ -1748,21 +1758,21 @@
         <v>43</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
       <c r="P10" s="2" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="Q10" s="2"/>
       <c r="R10" s="2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="S10" s="2"/>
       <c r="T10" s="2"/>
       <c r="U10" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="V10" s="2"/>
       <c r="W10" s="2"/>
@@ -1779,24 +1789,24 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2" t="s">
@@ -1812,16 +1822,16 @@
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
       <c r="P11" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="Q11" s="2"/>
       <c r="R11" s="2"/>
       <c r="S11" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="T11" s="2"/>
       <c r="U11" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="V11" s="2"/>
       <c r="W11" s="2"/>
@@ -1833,29 +1843,29 @@
       <c r="AC11" s="2"/>
       <c r="AD11" s="2"/>
       <c r="AE11" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2" t="s">
@@ -1871,15 +1881,15 @@
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
       <c r="P12" s="2" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="Q12" s="2"/>
       <c r="R12" s="2"/>
       <c r="S12" s="2" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="U12" s="2"/>
       <c r="V12" s="2"/>
@@ -1892,31 +1902,31 @@
       <c r="AC12" s="2"/>
       <c r="AD12" s="2"/>
       <c r="AE12" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>42</v>
@@ -1937,17 +1947,17 @@
       <c r="Q13" s="2"/>
       <c r="R13" s="2"/>
       <c r="S13" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="U13" s="2"/>
       <c r="V13" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
@@ -1962,29 +1972,29 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="J14" s="2" t="s">
         <v>43</v>
@@ -2005,7 +2015,7 @@
       <c r="T14" s="2"/>
       <c r="U14" s="2"/>
       <c r="V14" s="2" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="W14" s="2"/>
       <c r="X14" s="2"/>
@@ -2021,27 +2031,27 @@
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>34</v>
@@ -2056,12 +2066,12 @@
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
       <c r="P15" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="Q15" s="2"/>
       <c r="R15" s="2"/>
       <c r="S15" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T15" s="2"/>
       <c r="U15" s="2"/>
@@ -2080,27 +2090,27 @@
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>43</v>
@@ -2112,22 +2122,22 @@
         <v>43</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="O16" s="2"/>
       <c r="P16" s="2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
       <c r="S16" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
@@ -2138,16 +2148,16 @@
         <v>1</v>
       </c>
       <c r="AA16" s="2" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="AB16" s="2" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="AC16" s="2" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="AD16" s="2" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="AE16" s="2" t="s">
         <v>36</v>
@@ -2155,29 +2165,29 @@
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>43</v>
@@ -2189,24 +2199,24 @@
         <v>43</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="O17" s="2"/>
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
       <c r="R17" s="2"/>
       <c r="S17" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="U17" s="2"/>
       <c r="V17" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="W17" s="2"/>
       <c r="X17" s="2"/>
@@ -2215,7 +2225,7 @@
         <v>1</v>
       </c>
       <c r="AA17" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="AB17" s="2"/>
       <c r="AC17" s="2"/>
@@ -2226,29 +2236,29 @@
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>43</v>
@@ -2260,10 +2270,10 @@
         <v>43</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="O18" s="2"/>
       <c r="P18" s="2"/>
@@ -2271,11 +2281,11 @@
       <c r="R18" s="2"/>
       <c r="S18" s="2"/>
       <c r="T18" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="U18" s="2"/>
       <c r="V18" s="2" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="W18" s="2"/>
       <c r="X18" s="2"/>
@@ -2284,7 +2294,7 @@
         <v>1</v>
       </c>
       <c r="AA18" s="2" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="AB18" s="2"/>
       <c r="AC18" s="2"/>
@@ -2295,24 +2305,24 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>42</v>
@@ -2327,27 +2337,27 @@
         <v>43</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="O19" s="2"/>
       <c r="P19" s="2" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="Q19" s="2"/>
       <c r="R19" s="2" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="U19" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="V19" s="2"/>
       <c r="W19" s="2"/>
@@ -2355,7 +2365,7 @@
         <v>1</v>
       </c>
       <c r="Y19" s="2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
@@ -2368,24 +2378,24 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2" t="s">
@@ -2400,14 +2410,14 @@
       <c r="N20" s="2"/>
       <c r="O20" s="2"/>
       <c r="Q20" s="2" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="R20" s="2"/>
       <c r="S20" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="T20" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="U20" s="2"/>
       <c r="V20" s="2"/>
@@ -2416,7 +2426,7 @@
         <v>1</v>
       </c>
       <c r="Y20" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="Z20" s="2"/>
       <c r="AA20" s="2"/>
@@ -2429,24 +2439,24 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2" t="s">
@@ -2459,17 +2469,17 @@
         <v>43</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="N21" s="2"/>
       <c r="O21" s="2"/>
       <c r="Q21" s="2"/>
       <c r="R21" s="2"/>
       <c r="S21" s="2" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="T21" s="2" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="U21" s="2"/>
       <c r="V21" s="2"/>
@@ -2478,7 +2488,7 @@
         <v>1</v>
       </c>
       <c r="Y21" s="2" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="Z21" s="2"/>
       <c r="AA21" s="2"/>
@@ -2486,32 +2496,32 @@
       <c r="AC21" s="2"/>
       <c r="AD21" s="2"/>
       <c r="AE21" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="J22" s="2" t="s">
         <v>43</v>
@@ -2523,24 +2533,24 @@
         <v>43</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="O22" s="2"/>
       <c r="P22" s="2" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="Q22" s="2"/>
       <c r="R22" s="2" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="U22" s="2"/>
       <c r="V22" s="2"/>
@@ -2549,18 +2559,18 @@
         <v>1</v>
       </c>
       <c r="Y22" s="2" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="Z22" s="2"/>
       <c r="AA22" s="2"/>
       <c r="AB22" s="2" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="AC22" s="2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="AD22" s="2" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="AE22" s="2" t="s">
         <v>36</v>
@@ -2568,29 +2578,29 @@
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>43</v>
@@ -2602,27 +2612,27 @@
         <v>43</v>
       </c>
       <c r="M23" s="2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="O23" s="2"/>
       <c r="P23" s="2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="Q23" s="2"/>
       <c r="R23" s="2" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="S23" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T23" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="U23" s="2" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
@@ -2630,13 +2640,13 @@
         <v>1</v>
       </c>
       <c r="Y23" s="2" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="Z23" s="2"/>
       <c r="AA23" s="2"/>
       <c r="AB23" s="2"/>
       <c r="AC23" s="2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="AD23" s="2"/>
       <c r="AE23" s="2" t="s">
@@ -2645,27 +2655,27 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="E24" s="2"/>
       <c r="F24" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>34</v>
@@ -2677,25 +2687,25 @@
         <v>43</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="O24" s="2"/>
       <c r="P24" s="2" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="Q24" s="2"/>
       <c r="R24" s="2"/>
       <c r="S24" s="2" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="T24" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="U24" s="2" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="V24" s="2"/>
       <c r="W24" s="2"/>
@@ -2712,27 +2722,27 @@
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="E25" s="2"/>
       <c r="F25" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>34</v>
@@ -2744,19 +2754,19 @@
         <v>43</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="O25" s="2"/>
       <c r="P25" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="Q25" s="2"/>
       <c r="R25" s="2"/>
       <c r="S25" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T25" s="2"/>
       <c r="U25" s="2"/>
@@ -2775,24 +2785,24 @@
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>42</v>
@@ -2807,26 +2817,26 @@
         <v>43</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="O26" s="2"/>
       <c r="P26" s="2" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="S26" s="2" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="T26" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="U26" s="2"/>
       <c r="V26" s="2"/>
@@ -2835,7 +2845,7 @@
         <v>1</v>
       </c>
       <c r="Y26" s="2" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="Z26" s="2"/>
       <c r="AA26" s="2"/>
@@ -2848,24 +2858,24 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>42</v>
@@ -2880,26 +2890,26 @@
         <v>43</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" s="2" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="R27" s="2" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="S27" s="2" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="T27" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="U27" s="2"/>
       <c r="V27" s="2"/>
@@ -2908,7 +2918,7 @@
         <v>1</v>
       </c>
       <c r="Y27" s="2" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="Z27" s="2"/>
       <c r="AA27" s="2"/>
@@ -2921,24 +2931,24 @@
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="I28" s="2"/>
       <c r="J28" s="2" t="s">
@@ -2951,25 +2961,25 @@
         <v>43</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" s="2" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="Q28" s="2"/>
       <c r="R28" s="2"/>
       <c r="S28" s="2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="T28" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="U28" s="2" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="V28" s="2"/>
       <c r="W28" s="2"/>
@@ -2986,27 +2996,27 @@
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>43</v>
@@ -3018,22 +3028,22 @@
         <v>43</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="O29" s="2"/>
       <c r="P29" s="2" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="Q29" s="2"/>
       <c r="R29" s="2"/>
       <c r="S29" s="2" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="T29" s="2" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="U29" s="2"/>
       <c r="V29" s="2"/>
@@ -3042,12 +3052,12 @@
         <v>1</v>
       </c>
       <c r="Y29" s="2" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="Z29" s="2"/>
       <c r="AA29" s="2"/>
       <c r="AB29" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="AC29" s="2"/>
       <c r="AD29" s="2"/>
@@ -3057,27 +3067,27 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2" t="s">
         <v>33</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>43</v>
@@ -3089,19 +3099,19 @@
         <v>43</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="O30" s="2"/>
       <c r="P30" s="2"/>
       <c r="Q30" s="2" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="R30" s="2"/>
       <c r="S30" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="T30" s="2"/>
       <c r="U30" s="2"/>
@@ -3111,12 +3121,12 @@
         <v>1</v>
       </c>
       <c r="Y30" s="2" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="Z30" s="2"/>
       <c r="AA30" s="2"/>
       <c r="AB30" s="2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="AC30" s="2"/>
       <c r="AD30" s="2"/>

</xml_diff>